<commit_message>
add option item  sheets
</commit_message>
<xml_diff>
--- a/test/language.xlsx
+++ b/test/language.xlsx
@@ -5,14 +5,14 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="2" r:id="rId5"/>
+    <sheet name="sheet_1" sheetId="1" r:id="rId4"/>
+    <sheet name="SHEET_2" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>key</t>
   </si>
@@ -58,6 +58,15 @@
   <si>
     <t>创建图标 title</t>
   </si>
+  <si>
+    <t>表格 1</t>
+  </si>
+  <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>menu.new1</t>
+  </si>
 </sst>
 </file>
 
@@ -75,7 +84,7 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica"/>
+      <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="14"/>
@@ -83,7 +92,7 @@
       <name val="宋体"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,8 +105,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -165,13 +186,190 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -190,10 +388,79 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -216,6 +483,10 @@
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff7f7f7f"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -264,14 +535,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office 主题​​">
       <a:majorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office 主题​​">
@@ -479,7 +750,7 @@
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1056,7 +1327,7 @@
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1307,22 +1578,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71429" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.66667" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="28.1562" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1562" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7344" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5781" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.73438" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.73438" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.73438" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.73438" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.73438" style="1" customWidth="1"/>
-    <col min="10" max="256" width="8.73438" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1719" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.8516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.6719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85156" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85156" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85156" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85156" style="1" customWidth="1"/>
+    <col min="10" max="256" width="8.67188" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="21.25" customHeight="1">
@@ -1421,106 +1692,209 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
+    <row r="7" ht="16" customHeight="1">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" ht="16" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" ht="16" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" ht="16" customHeight="1">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="14"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71429" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.73438" style="6" customWidth="1"/>
-    <col min="2" max="2" width="8.73438" style="6" customWidth="1"/>
-    <col min="3" max="3" width="8.73438" style="6" customWidth="1"/>
-    <col min="4" max="4" width="8.73438" style="6" customWidth="1"/>
-    <col min="5" max="5" width="8.73438" style="6" customWidth="1"/>
-    <col min="6" max="256" width="8.73438" style="6" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="15" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="15" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="15" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="15" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="15" customWidth="1"/>
+    <col min="6" max="6" width="16.3516" style="15" customWidth="1"/>
+    <col min="7" max="256" width="16.3516" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16" customHeight="1">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+    <row r="1" ht="20" customHeight="1">
+      <c r="A1" t="s" s="16">
+        <v>15</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" ht="16" customHeight="1">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="A2" t="s" s="17">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s" s="17">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s" s="17">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s" s="17">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s" s="18">
+        <v>4</v>
+      </c>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" ht="16" customHeight="1">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="A3" t="s" s="19">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s" s="20">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s" s="20">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s" s="20">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s" s="20">
+        <v>9</v>
+      </c>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" ht="16" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="A4" t="s" s="21">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s" s="22">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s" s="22">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s" s="22">
+        <v>14</v>
+      </c>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" ht="16" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" ht="16" customHeight="1">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" ht="16" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" ht="16" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" ht="16" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+    </row>
+    <row r="7" ht="15.65" customHeight="1">
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+    </row>
+    <row r="8" ht="15.35" customHeight="1">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+    </row>
+    <row r="9" ht="15.35" customHeight="1">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+    </row>
+    <row r="10" ht="15.35" customHeight="1">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+    </row>
+    <row r="11" ht="15.35" customHeight="1">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>